<commit_message>
add parton to hadron level correction and update note
</commit_message>
<xml_diff>
--- a/jets/expdata/10001.xlsx
+++ b/jets/expdata/10001.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
   <si>
     <t>idx</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>%-sys23_c</t>
+  </si>
+  <si>
+    <t>%-parton-to-hadron</t>
   </si>
   <si>
     <t>plot-factor</t>
@@ -772,15 +775,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1102,12 +1102,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AN123"/>
+  <dimension ref="A1:AO123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" topLeftCell="AH1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="AN1" sqref="AN$1:AN$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71120689655172" defaultRowHeight="24.4"/>
@@ -1140,11 +1140,12 @@
     <col min="36" max="36" width="13.5689655172414" customWidth="1"/>
     <col min="37" max="37" width="12.8534482758621" customWidth="1"/>
     <col min="38" max="39" width="13.2844827586207" customWidth="1"/>
-    <col min="40" max="40" width="13.1422413793103" customWidth="1"/>
-    <col min="41" max="1026" width="10.2844827586207" customWidth="1"/>
+    <col min="40" max="40" width="23.5862068965517" customWidth="1"/>
+    <col min="41" max="41" width="13.1422413793103" customWidth="1"/>
+    <col min="42" max="1027" width="10.2844827586207" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="35.6" spans="1:40">
+    <row r="1" ht="35.6" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,16 +1266,19 @@
       <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" ht="35.6" spans="1:40">
+    <row r="2" ht="35.6" spans="1:41">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1">
         <v>1960</v>
@@ -1302,10 +1306,10 @@
         <v>0.7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N2" s="2">
         <v>23143</v>
@@ -1386,18 +1390,21 @@
         <v>0.1</v>
       </c>
       <c r="AN2" s="1">
+        <v>111.3</v>
+      </c>
+      <c r="AO2" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="3" ht="35.6" spans="1:40">
+    <row r="3" ht="35.6" spans="1:41">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1">
         <v>1960</v>
@@ -1425,10 +1432,10 @@
         <v>0.7</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N3" s="2">
         <v>8818</v>
@@ -1509,18 +1516,21 @@
         <v>0.2</v>
       </c>
       <c r="AN3" s="1">
+        <v>109.8</v>
+      </c>
+      <c r="AO3" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="4" ht="35.6" spans="1:40">
+    <row r="4" ht="35.6" spans="1:41">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1">
         <v>1960</v>
@@ -1548,10 +1558,10 @@
         <v>0.7</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N4" s="2">
         <v>3772</v>
@@ -1632,18 +1642,21 @@
         <v>0.3</v>
       </c>
       <c r="AN4" s="1">
+        <v>108.5</v>
+      </c>
+      <c r="AO4" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="5" ht="35.6" spans="1:40">
+    <row r="5" ht="35.6" spans="1:41">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1">
         <v>1960</v>
@@ -1671,10 +1684,10 @@
         <v>0.7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5" s="2">
         <v>1759</v>
@@ -1755,18 +1768,21 @@
         <v>0.3</v>
       </c>
       <c r="AN5" s="1">
+        <v>107.5</v>
+      </c>
+      <c r="AO5" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="6" ht="35.6" spans="1:40">
+    <row r="6" ht="35.6" spans="1:41">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1">
         <v>1960</v>
@@ -1794,10 +1810,10 @@
         <v>0.7</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N6" s="2">
         <v>893</v>
@@ -1878,18 +1894,21 @@
         <v>0.4</v>
       </c>
       <c r="AN6" s="1">
+        <v>106.6</v>
+      </c>
+      <c r="AO6" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="7" ht="35.6" spans="1:40">
+    <row r="7" ht="35.6" spans="1:41">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>1960</v>
@@ -1917,10 +1936,10 @@
         <v>0.7</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N7" s="2">
         <v>482.8</v>
@@ -2001,18 +2020,21 @@
         <v>0.4</v>
       </c>
       <c r="AN7" s="1">
+        <v>105.9</v>
+      </c>
+      <c r="AO7" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="8" ht="35.6" spans="1:40">
+    <row r="8" ht="35.6" spans="1:41">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1">
         <v>1960</v>
@@ -2040,10 +2062,10 @@
         <v>0.7</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N8" s="2">
         <v>274.4</v>
@@ -2124,18 +2146,21 @@
         <v>0.4</v>
       </c>
       <c r="AN8" s="1">
+        <v>105.3</v>
+      </c>
+      <c r="AO8" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="9" ht="35.6" spans="1:40">
+    <row r="9" ht="35.6" spans="1:41">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1">
         <v>1960</v>
@@ -2163,10 +2188,10 @@
         <v>0.7</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N9" s="2">
         <v>158.8</v>
@@ -2247,18 +2272,21 @@
         <v>0.4</v>
       </c>
       <c r="AN9" s="1">
+        <v>104.8</v>
+      </c>
+      <c r="AO9" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="10" ht="35.6" spans="1:40">
+    <row r="10" ht="35.6" spans="1:41">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1">
         <v>1960</v>
@@ -2286,10 +2314,10 @@
         <v>0.7</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N10" s="2">
         <v>86.44</v>
@@ -2370,18 +2398,21 @@
         <v>0.4</v>
       </c>
       <c r="AN10" s="1">
+        <v>104.3</v>
+      </c>
+      <c r="AO10" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="11" ht="35.6" spans="1:40">
+    <row r="11" ht="35.6" spans="1:41">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1">
         <v>1960</v>
@@ -2409,10 +2440,10 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N11" s="2">
         <v>43.38</v>
@@ -2493,18 +2524,21 @@
         <v>0.4</v>
       </c>
       <c r="AN11" s="1">
+        <v>103.8</v>
+      </c>
+      <c r="AO11" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="35.6" spans="1:40">
+    <row r="12" ht="35.6" spans="1:41">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1">
         <v>1960</v>
@@ -2532,10 +2566,10 @@
         <v>0.7</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N12" s="2">
         <v>21.31</v>
@@ -2616,18 +2650,21 @@
         <v>0.4</v>
       </c>
       <c r="AN12" s="1">
+        <v>103.4</v>
+      </c>
+      <c r="AO12" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="13" ht="35.6" spans="1:40">
+    <row r="13" ht="35.6" spans="1:41">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1">
         <v>1960</v>
@@ -2655,10 +2692,10 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N13" s="2">
         <v>9.81</v>
@@ -2739,18 +2776,21 @@
         <v>0.4</v>
       </c>
       <c r="AN13" s="1">
+        <v>103.1</v>
+      </c>
+      <c r="AO13" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="14" ht="35.6" spans="1:40">
+    <row r="14" ht="35.6" spans="1:41">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1">
         <v>1960</v>
@@ -2778,10 +2818,10 @@
         <v>0.7</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N14" s="2">
         <v>4.719</v>
@@ -2862,18 +2902,21 @@
         <v>0.3</v>
       </c>
       <c r="AN14" s="1">
+        <v>102.9</v>
+      </c>
+      <c r="AO14" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="15" ht="35.6" spans="1:40">
+    <row r="15" ht="35.6" spans="1:41">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1">
         <v>1960</v>
@@ -2901,10 +2944,10 @@
         <v>0.7</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N15" s="2">
         <v>2.417</v>
@@ -2985,18 +3028,21 @@
         <v>0.3</v>
       </c>
       <c r="AN15" s="1">
+        <v>102.7</v>
+      </c>
+      <c r="AO15" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="16" ht="35.6" spans="1:40">
+    <row r="16" ht="35.6" spans="1:41">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1">
         <v>1960</v>
@@ -3024,10 +3070,10 @@
         <v>0.7</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N16" s="2">
         <v>1.177</v>
@@ -3108,18 +3154,21 @@
         <v>0.2</v>
       </c>
       <c r="AN16" s="1">
+        <v>102.6</v>
+      </c>
+      <c r="AO16" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="17" ht="35.6" spans="1:40">
+    <row r="17" ht="35.6" spans="1:41">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1">
         <v>1960</v>
@@ -3147,10 +3196,10 @@
         <v>0.7</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N17" s="2">
         <v>0.5084</v>
@@ -3231,18 +3280,21 @@
         <v>0.1</v>
       </c>
       <c r="AN17" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="AO17" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="18" ht="35.6" spans="1:40">
+    <row r="18" ht="35.6" spans="1:41">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1">
         <v>1960</v>
@@ -3270,10 +3322,10 @@
         <v>0.7</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N18" s="2">
         <v>0.2097</v>
@@ -3354,18 +3406,21 @@
         <v>0.1</v>
       </c>
       <c r="AN18" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="AO18" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="19" ht="35.6" spans="1:40">
+    <row r="19" ht="35.6" spans="1:41">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1">
         <v>1960</v>
@@ -3393,10 +3448,10 @@
         <v>0.7</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N19" s="2">
         <v>0.08189</v>
@@ -3477,18 +3532,21 @@
         <v>0.3</v>
       </c>
       <c r="AN19" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="AO19" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="20" ht="35.6" spans="1:40">
+    <row r="20" ht="35.6" spans="1:41">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1">
         <v>1960</v>
@@ -3516,10 +3574,10 @@
         <v>0.7</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N20" s="2">
         <v>0.02909</v>
@@ -3600,18 +3658,21 @@
         <v>0.5</v>
       </c>
       <c r="AN20" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="AO20" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="21" ht="35.6" spans="1:40">
+    <row r="21" ht="35.6" spans="1:41">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1">
         <v>1960</v>
@@ -3639,10 +3700,10 @@
         <v>0.7</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N21" s="2">
         <v>0.009915</v>
@@ -3723,18 +3784,21 @@
         <v>0.9</v>
       </c>
       <c r="AN21" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO21" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="22" ht="35.6" spans="1:40">
+    <row r="22" ht="35.6" spans="1:41">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1">
         <v>1960</v>
@@ -3762,10 +3826,10 @@
         <v>0.7</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N22" s="2">
         <v>0.003032</v>
@@ -3846,18 +3910,21 @@
         <v>1.4</v>
       </c>
       <c r="AN22" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO22" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="23" ht="35.6" spans="1:40">
+    <row r="23" ht="35.6" spans="1:41">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1">
         <v>1960</v>
@@ -3885,10 +3952,10 @@
         <v>0.7</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N23" s="2">
         <v>0.0005925</v>
@@ -3969,18 +4036,21 @@
         <v>2.1</v>
       </c>
       <c r="AN23" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO23" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="24" ht="35.6" spans="1:40">
+    <row r="24" ht="35.6" spans="1:41">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1">
         <v>1960</v>
@@ -4008,102 +4078,105 @@
         <v>0.7</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N24" s="2">
         <v>8.917e-5</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="1">
         <v>3.638e-5</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24" s="1">
         <v>3.1</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24" s="1">
         <v>8</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24" s="1">
         <v>12.5</v>
       </c>
-      <c r="S24" s="3">
+      <c r="S24" s="1">
         <v>10.6</v>
       </c>
-      <c r="T24" s="3">
-        <v>0</v>
-      </c>
-      <c r="U24" s="3">
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
         <v>8</v>
       </c>
-      <c r="V24" s="3">
+      <c r="V24" s="1">
         <v>6.5</v>
       </c>
-      <c r="W24" s="3">
+      <c r="W24" s="1">
         <v>1.5</v>
       </c>
-      <c r="X24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="3">
+      <c r="X24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="1">
         <v>1</v>
       </c>
-      <c r="AA24" s="3">
+      <c r="AA24" s="1">
         <v>0.2</v>
       </c>
-      <c r="AB24" s="3">
+      <c r="AB24" s="1">
         <v>0.1</v>
       </c>
-      <c r="AC24" s="3">
+      <c r="AC24" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD24" s="3">
+      <c r="AD24" s="1">
         <v>2.4</v>
       </c>
-      <c r="AE24" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="3">
+      <c r="AE24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
         <v>5.5</v>
       </c>
-      <c r="AG24" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="3">
+      <c r="AG24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="1">
         <v>0.9</v>
       </c>
-      <c r="AJ24" s="3">
+      <c r="AJ24" s="1">
         <v>1.5</v>
       </c>
-      <c r="AK24" s="3">
+      <c r="AK24" s="1">
         <v>1.2</v>
       </c>
-      <c r="AL24" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="3">
+      <c r="AL24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="1">
         <v>3.3</v>
       </c>
       <c r="AN24" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO24" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="25" ht="35.6" spans="1:40">
+    <row r="25" ht="35.6" spans="1:41">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="1">
         <v>1960</v>
@@ -4131,10 +4204,10 @@
         <v>0.7</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N25" s="2">
         <v>21566</v>
@@ -4215,18 +4288,21 @@
         <v>0.1</v>
       </c>
       <c r="AN25" s="1">
+        <v>111.9</v>
+      </c>
+      <c r="AO25" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="26" ht="35.6" spans="1:40">
+    <row r="26" ht="35.6" spans="1:41">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1">
         <v>1960</v>
@@ -4254,10 +4330,10 @@
         <v>0.7</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N26" s="2">
         <v>8106</v>
@@ -4338,18 +4414,21 @@
         <v>0.2</v>
       </c>
       <c r="AN26" s="1">
+        <v>110.2</v>
+      </c>
+      <c r="AO26" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="27" ht="35.6" spans="1:40">
+    <row r="27" ht="35.6" spans="1:41">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1">
         <v>1960</v>
@@ -4377,10 +4456,10 @@
         <v>0.7</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N27" s="2">
         <v>3471</v>
@@ -4461,18 +4540,21 @@
         <v>0.3</v>
       </c>
       <c r="AN27" s="1">
+        <v>108.9</v>
+      </c>
+      <c r="AO27" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="28" ht="35.6" spans="1:40">
+    <row r="28" ht="35.6" spans="1:41">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D28" s="1">
         <v>1960</v>
@@ -4500,10 +4582,10 @@
         <v>0.7</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N28" s="2">
         <v>1611</v>
@@ -4584,18 +4666,21 @@
         <v>0.3</v>
       </c>
       <c r="AN28" s="1">
+        <v>107.7</v>
+      </c>
+      <c r="AO28" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="29" ht="35.6" spans="1:40">
+    <row r="29" ht="35.6" spans="1:41">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1">
         <v>1960</v>
@@ -4623,10 +4708,10 @@
         <v>0.7</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N29" s="2">
         <v>799.8</v>
@@ -4707,18 +4792,21 @@
         <v>0.4</v>
       </c>
       <c r="AN29" s="1">
+        <v>106.8</v>
+      </c>
+      <c r="AO29" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="30" ht="35.6" spans="1:40">
+    <row r="30" ht="35.6" spans="1:41">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1">
         <v>1960</v>
@@ -4746,10 +4834,10 @@
         <v>0.7</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N30" s="2">
         <v>435.3</v>
@@ -4830,18 +4918,21 @@
         <v>0.4</v>
       </c>
       <c r="AN30" s="1">
+        <v>106</v>
+      </c>
+      <c r="AO30" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="31" ht="35.6" spans="1:40">
+    <row r="31" ht="35.6" spans="1:41">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D31" s="1">
         <v>1960</v>
@@ -4869,10 +4960,10 @@
         <v>0.7</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N31" s="2">
         <v>241.5</v>
@@ -4953,18 +5044,21 @@
         <v>0.4</v>
       </c>
       <c r="AN31" s="1">
+        <v>105.4</v>
+      </c>
+      <c r="AO31" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="32" ht="35.6" spans="1:40">
+    <row r="32" ht="35.6" spans="1:41">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1">
         <v>1960</v>
@@ -4992,10 +5086,10 @@
         <v>0.7</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N32" s="2">
         <v>140.9</v>
@@ -5076,18 +5170,21 @@
         <v>0.4</v>
       </c>
       <c r="AN32" s="1">
+        <v>104.8</v>
+      </c>
+      <c r="AO32" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="33" ht="35.6" spans="1:40">
+    <row r="33" ht="35.6" spans="1:41">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D33" s="1">
         <v>1960</v>
@@ -5115,10 +5212,10 @@
         <v>0.7</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N33" s="2">
         <v>76.38</v>
@@ -5199,18 +5296,21 @@
         <v>0.4</v>
       </c>
       <c r="AN33" s="1">
+        <v>104.3</v>
+      </c>
+      <c r="AO33" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="34" ht="35.6" spans="1:40">
+    <row r="34" ht="35.6" spans="1:41">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1">
         <v>1960</v>
@@ -5238,10 +5338,10 @@
         <v>0.7</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N34" s="2">
         <v>38.05</v>
@@ -5322,18 +5422,21 @@
         <v>0.4</v>
       </c>
       <c r="AN34" s="1">
+        <v>103.8</v>
+      </c>
+      <c r="AO34" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="35" ht="35.6" spans="1:40">
+    <row r="35" ht="35.6" spans="1:41">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D35" s="1">
         <v>1960</v>
@@ -5361,10 +5464,10 @@
         <v>0.7</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N35" s="2">
         <v>18.11</v>
@@ -5445,18 +5548,21 @@
         <v>0.4</v>
       </c>
       <c r="AN35" s="1">
+        <v>103.4</v>
+      </c>
+      <c r="AO35" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="36" ht="35.6" spans="1:40">
+    <row r="36" ht="35.6" spans="1:41">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D36" s="1">
         <v>1960</v>
@@ -5484,10 +5590,10 @@
         <v>0.7</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N36" s="2">
         <v>8.105</v>
@@ -5568,18 +5674,21 @@
         <v>0.4</v>
       </c>
       <c r="AN36" s="1">
+        <v>103.1</v>
+      </c>
+      <c r="AO36" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="37" ht="35.6" spans="1:40">
+    <row r="37" ht="35.6" spans="1:41">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D37" s="1">
         <v>1960</v>
@@ -5607,10 +5716,10 @@
         <v>0.7</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N37" s="2">
         <v>3.779</v>
@@ -5691,18 +5800,21 @@
         <v>0.3</v>
       </c>
       <c r="AN37" s="1">
+        <v>102.8</v>
+      </c>
+      <c r="AO37" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="38" ht="35.6" spans="1:40">
+    <row r="38" ht="35.6" spans="1:41">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D38" s="1">
         <v>1960</v>
@@ -5730,10 +5842,10 @@
         <v>0.7</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N38" s="2">
         <v>1.853</v>
@@ -5814,18 +5926,21 @@
         <v>0.3</v>
       </c>
       <c r="AN38" s="1">
+        <v>102.7</v>
+      </c>
+      <c r="AO38" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="39" ht="35.6" spans="1:40">
+    <row r="39" ht="35.6" spans="1:41">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D39" s="1">
         <v>1960</v>
@@ -5853,10 +5968,10 @@
         <v>0.7</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N39" s="2">
         <v>0.8718</v>
@@ -5937,18 +6052,21 @@
         <v>0.2</v>
       </c>
       <c r="AN39" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="AO39" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="40" ht="35.6" spans="1:40">
+    <row r="40" ht="35.6" spans="1:41">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D40" s="1">
         <v>1960</v>
@@ -5976,10 +6094,10 @@
         <v>0.7</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N40" s="2">
         <v>0.3532</v>
@@ -6060,18 +6178,21 @@
         <v>0.1</v>
       </c>
       <c r="AN40" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="AO40" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="41" ht="35.6" spans="1:40">
+    <row r="41" ht="35.6" spans="1:41">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D41" s="1">
         <v>1960</v>
@@ -6099,10 +6220,10 @@
         <v>0.7</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N41" s="2">
         <v>0.1381</v>
@@ -6183,18 +6304,21 @@
         <v>0.1</v>
       </c>
       <c r="AN41" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="AO41" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="42" ht="35.6" spans="1:40">
+    <row r="42" ht="35.6" spans="1:41">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="1">
         <v>1960</v>
@@ -6222,10 +6346,10 @@
         <v>0.7</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N42" s="2">
         <v>0.0527</v>
@@ -6306,18 +6430,21 @@
         <v>0.3</v>
       </c>
       <c r="AN42" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="AO42" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="43" ht="35.6" spans="1:40">
+    <row r="43" ht="35.6" spans="1:41">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D43" s="1">
         <v>1960</v>
@@ -6345,10 +6472,10 @@
         <v>0.7</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N43" s="2">
         <v>0.01539</v>
@@ -6429,18 +6556,21 @@
         <v>0.7</v>
       </c>
       <c r="AN43" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO43" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="44" ht="35.6" spans="1:40">
+    <row r="44" ht="35.6" spans="1:41">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D44" s="1">
         <v>1960</v>
@@ -6468,10 +6598,10 @@
         <v>0.7</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N44" s="2">
         <v>0.003741</v>
@@ -6552,18 +6682,21 @@
         <v>1.1</v>
       </c>
       <c r="AN44" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO44" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="45" ht="35.6" spans="1:40">
+    <row r="45" ht="35.6" spans="1:41">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D45" s="1">
         <v>1960</v>
@@ -6591,10 +6724,10 @@
         <v>0.7</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N45" s="2">
         <v>0.0007379</v>
@@ -6675,18 +6808,21 @@
         <v>1.8</v>
       </c>
       <c r="AN45" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO45" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="46" ht="35.6" spans="1:40">
+    <row r="46" ht="35.6" spans="1:41">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D46" s="1">
         <v>1960</v>
@@ -6714,102 +6850,105 @@
         <v>0.7</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N46" s="2">
         <v>6.021e-5</v>
       </c>
-      <c r="O46" s="3">
+      <c r="O46" s="1">
         <v>2.457e-5</v>
       </c>
-      <c r="P46" s="3">
+      <c r="P46" s="1">
         <v>3.7</v>
       </c>
-      <c r="Q46" s="3">
+      <c r="Q46" s="1">
         <v>8.6</v>
       </c>
-      <c r="R46" s="3">
+      <c r="R46" s="1">
         <v>13.4</v>
       </c>
-      <c r="S46" s="3">
+      <c r="S46" s="1">
         <v>11.3</v>
       </c>
-      <c r="T46" s="3">
-        <v>0</v>
-      </c>
-      <c r="U46" s="3">
+      <c r="T46" s="1">
+        <v>0</v>
+      </c>
+      <c r="U46" s="1">
         <v>9</v>
       </c>
-      <c r="V46" s="3">
+      <c r="V46" s="1">
         <v>6.5</v>
       </c>
-      <c r="W46" s="3">
+      <c r="W46" s="1">
         <v>8</v>
       </c>
-      <c r="X46" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="3">
+      <c r="X46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="1">
         <v>2.4</v>
       </c>
-      <c r="AA46" s="3">
+      <c r="AA46" s="1">
         <v>2.6</v>
       </c>
-      <c r="AB46" s="3">
+      <c r="AB46" s="1">
         <v>0.1</v>
       </c>
-      <c r="AC46" s="3">
+      <c r="AC46" s="1">
         <v>1.7</v>
       </c>
-      <c r="AD46" s="3">
+      <c r="AD46" s="1">
         <v>3.1</v>
       </c>
-      <c r="AE46" s="3">
+      <c r="AE46" s="1">
         <v>3.4</v>
       </c>
-      <c r="AF46" s="3">
+      <c r="AF46" s="1">
         <v>6</v>
       </c>
-      <c r="AG46" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH46" s="3">
+      <c r="AG46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="1">
         <v>0.3</v>
       </c>
-      <c r="AI46" s="3">
+      <c r="AI46" s="1">
         <v>0.9</v>
       </c>
-      <c r="AJ46" s="3">
+      <c r="AJ46" s="1">
         <v>1.8</v>
       </c>
-      <c r="AK46" s="3">
+      <c r="AK46" s="1">
         <v>1.3</v>
       </c>
-      <c r="AL46" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM46" s="3">
+      <c r="AL46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="1">
         <v>3</v>
       </c>
       <c r="AN46" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO46" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="47" ht="35.6" spans="1:40">
+    <row r="47" ht="35.6" spans="1:41">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D47" s="1">
         <v>1960</v>
@@ -6837,10 +6976,10 @@
         <v>0.7</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N47" s="2">
         <v>17563</v>
@@ -6921,18 +7060,21 @@
         <v>0.1</v>
       </c>
       <c r="AN47" s="1">
+        <v>113.5</v>
+      </c>
+      <c r="AO47" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="48" ht="35.6" spans="1:40">
+    <row r="48" ht="35.6" spans="1:41">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D48" s="1">
         <v>1960</v>
@@ -6960,10 +7102,10 @@
         <v>0.7</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N48" s="2">
         <v>6579</v>
@@ -7044,18 +7186,21 @@
         <v>0.2</v>
       </c>
       <c r="AN48" s="1">
+        <v>111.4</v>
+      </c>
+      <c r="AO48" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="49" ht="35.6" spans="1:40">
+    <row r="49" ht="35.6" spans="1:41">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D49" s="1">
         <v>1960</v>
@@ -7083,10 +7228,10 @@
         <v>0.7</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N49" s="2">
         <v>2786</v>
@@ -7167,18 +7312,21 @@
         <v>0.3</v>
       </c>
       <c r="AN49" s="1">
+        <v>109.7</v>
+      </c>
+      <c r="AO49" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="50" ht="35.6" spans="1:40">
+    <row r="50" ht="35.6" spans="1:41">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D50" s="1">
         <v>1960</v>
@@ -7206,10 +7354,10 @@
         <v>0.7</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N50" s="2">
         <v>1283</v>
@@ -7290,18 +7438,21 @@
         <v>0.3</v>
       </c>
       <c r="AN50" s="1">
+        <v>108.3</v>
+      </c>
+      <c r="AO50" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="51" ht="35.6" spans="1:40">
+    <row r="51" ht="35.6" spans="1:41">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D51" s="1">
         <v>1960</v>
@@ -7329,10 +7480,10 @@
         <v>0.7</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N51" s="2">
         <v>654</v>
@@ -7413,18 +7564,21 @@
         <v>0.4</v>
       </c>
       <c r="AN51" s="1">
+        <v>107.1</v>
+      </c>
+      <c r="AO51" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="52" ht="35.6" spans="1:40">
+    <row r="52" ht="35.6" spans="1:41">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D52" s="1">
         <v>1960</v>
@@ -7452,10 +7606,10 @@
         <v>0.7</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N52" s="2">
         <v>338</v>
@@ -7536,18 +7690,21 @@
         <v>0.4</v>
       </c>
       <c r="AN52" s="1">
+        <v>106.2</v>
+      </c>
+      <c r="AO52" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="53" ht="35.6" spans="1:40">
+    <row r="53" ht="35.6" spans="1:41">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D53" s="1">
         <v>1960</v>
@@ -7575,10 +7732,10 @@
         <v>0.7</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N53" s="2">
         <v>169</v>
@@ -7659,18 +7816,21 @@
         <v>0.4</v>
       </c>
       <c r="AN53" s="1">
+        <v>105.4</v>
+      </c>
+      <c r="AO53" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="54" ht="35.6" spans="1:40">
+    <row r="54" ht="35.6" spans="1:41">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D54" s="1">
         <v>1960</v>
@@ -7698,10 +7858,10 @@
         <v>0.7</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N54" s="2">
         <v>74.54</v>
@@ -7782,18 +7942,21 @@
         <v>0.5</v>
       </c>
       <c r="AN54" s="1">
+        <v>104.5</v>
+      </c>
+      <c r="AO54" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="55" ht="35.6" spans="1:40">
+    <row r="55" ht="35.6" spans="1:41">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D55" s="1">
         <v>1960</v>
@@ -7821,10 +7984,10 @@
         <v>0.7</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N55" s="2">
         <v>36.13</v>
@@ -7905,18 +8068,21 @@
         <v>0.5</v>
       </c>
       <c r="AN55" s="1">
+        <v>103.9</v>
+      </c>
+      <c r="AO55" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="56" ht="35.6" spans="1:40">
+    <row r="56" ht="35.6" spans="1:41">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D56" s="1">
         <v>1960</v>
@@ -7944,10 +8110,10 @@
         <v>0.7</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N56" s="2">
         <v>17.94</v>
@@ -8028,18 +8194,21 @@
         <v>0.5</v>
       </c>
       <c r="AN56" s="1">
+        <v>103.5</v>
+      </c>
+      <c r="AO56" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="57" ht="35.6" spans="1:40">
+    <row r="57" ht="35.6" spans="1:41">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D57" s="1">
         <v>1960</v>
@@ -8067,10 +8236,10 @@
         <v>0.7</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N57" s="2">
         <v>8.458</v>
@@ -8151,18 +8320,21 @@
         <v>0.4</v>
       </c>
       <c r="AN57" s="1">
+        <v>103.1</v>
+      </c>
+      <c r="AO57" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="58" ht="35.6" spans="1:40">
+    <row r="58" ht="35.6" spans="1:41">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D58" s="1">
         <v>1960</v>
@@ -8190,10 +8362,10 @@
         <v>0.7</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N58" s="2">
         <v>3.641</v>
@@ -8274,18 +8446,21 @@
         <v>0.4</v>
       </c>
       <c r="AN58" s="1">
+        <v>102.8</v>
+      </c>
+      <c r="AO58" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="59" ht="35.6" spans="1:40">
+    <row r="59" ht="35.6" spans="1:41">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D59" s="1">
         <v>1960</v>
@@ -8313,10 +8488,10 @@
         <v>0.7</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N59" s="2">
         <v>1.633</v>
@@ -8397,18 +8572,21 @@
         <v>0.3</v>
       </c>
       <c r="AN59" s="1">
+        <v>102.6</v>
+      </c>
+      <c r="AO59" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="60" ht="35.6" spans="1:40">
+    <row r="60" ht="35.6" spans="1:41">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D60" s="1">
         <v>1960</v>
@@ -8436,10 +8614,10 @@
         <v>0.7</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N60" s="2">
         <v>0.757</v>
@@ -8520,18 +8698,21 @@
         <v>0.3</v>
       </c>
       <c r="AN60" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="AO60" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="61" ht="35.6" spans="1:40">
+    <row r="61" ht="35.6" spans="1:41">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D61" s="1">
         <v>1960</v>
@@ -8559,10 +8740,10 @@
         <v>0.7</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N61" s="2">
         <v>0.3551</v>
@@ -8643,18 +8824,21 @@
         <v>0.2</v>
       </c>
       <c r="AN61" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="AO61" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="62" ht="35.6" spans="1:40">
+    <row r="62" ht="35.6" spans="1:41">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D62" s="1">
         <v>1960</v>
@@ -8682,10 +8866,10 @@
         <v>0.7</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N62" s="2">
         <v>0.143</v>
@@ -8766,18 +8950,21 @@
         <v>0</v>
       </c>
       <c r="AN62" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO62" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="63" ht="35.6" spans="1:40">
+    <row r="63" ht="35.6" spans="1:41">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D63" s="1">
         <v>1960</v>
@@ -8805,10 +8992,10 @@
         <v>0.7</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N63" s="2">
         <v>0.04104</v>
@@ -8889,18 +9076,21 @@
         <v>0.2</v>
       </c>
       <c r="AN63" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO63" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="64" ht="35.6" spans="1:40">
+    <row r="64" ht="35.6" spans="1:41">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D64" s="1">
         <v>1960</v>
@@ -8928,10 +9118,10 @@
         <v>0.7</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N64" s="2">
         <v>0.0103</v>
@@ -9012,18 +9202,21 @@
         <v>0.5</v>
       </c>
       <c r="AN64" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO64" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="65" ht="35.6" spans="1:40">
+    <row r="65" ht="35.6" spans="1:41">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D65" s="1">
         <v>1960</v>
@@ -9051,10 +9244,10 @@
         <v>0.7</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N65" s="2">
         <v>0.002388</v>
@@ -9135,18 +9328,21 @@
         <v>1</v>
       </c>
       <c r="AN65" s="1">
+        <v>102.2</v>
+      </c>
+      <c r="AO65" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="66" ht="35.6" spans="1:40">
+    <row r="66" ht="35.6" spans="1:41">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D66" s="1">
         <v>1960</v>
@@ -9174,102 +9370,105 @@
         <v>0.7</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N66" s="2">
         <v>0.0001565</v>
       </c>
-      <c r="O66" s="3">
+      <c r="O66" s="1">
         <v>3.07e-5</v>
       </c>
-      <c r="P66" s="3">
+      <c r="P66" s="1">
         <v>7.1</v>
       </c>
-      <c r="Q66" s="3">
+      <c r="Q66" s="1">
         <v>8</v>
       </c>
-      <c r="R66" s="3">
+      <c r="R66" s="1">
         <v>12.6</v>
       </c>
-      <c r="S66" s="3">
+      <c r="S66" s="1">
         <v>10.8</v>
       </c>
-      <c r="T66" s="3">
-        <v>0</v>
-      </c>
-      <c r="U66" s="3">
+      <c r="T66" s="1">
+        <v>0</v>
+      </c>
+      <c r="U66" s="1">
         <v>8.8</v>
       </c>
-      <c r="V66" s="3">
+      <c r="V66" s="1">
         <v>6.5</v>
       </c>
-      <c r="W66" s="3">
+      <c r="W66" s="1">
         <v>11.6</v>
       </c>
-      <c r="X66" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="3">
+      <c r="X66" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="1">
         <v>4.3</v>
       </c>
-      <c r="AA66" s="3">
+      <c r="AA66" s="1">
         <v>10.9</v>
       </c>
-      <c r="AB66" s="3">
+      <c r="AB66" s="1">
         <v>5.9</v>
       </c>
-      <c r="AC66" s="3">
+      <c r="AC66" s="1">
         <v>2</v>
       </c>
-      <c r="AD66" s="3">
+      <c r="AD66" s="1">
         <v>5.9</v>
       </c>
-      <c r="AE66" s="3">
+      <c r="AE66" s="1">
         <v>3.1</v>
       </c>
-      <c r="AF66" s="3">
+      <c r="AF66" s="1">
         <v>3.3</v>
       </c>
-      <c r="AG66" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH66" s="3">
+      <c r="AG66" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="1">
         <v>0.8</v>
       </c>
-      <c r="AI66" s="3">
+      <c r="AI66" s="1">
         <v>1.4</v>
       </c>
-      <c r="AJ66" s="3">
+      <c r="AJ66" s="1">
         <v>1.6</v>
       </c>
-      <c r="AK66" s="3">
+      <c r="AK66" s="1">
         <v>1.4</v>
       </c>
-      <c r="AL66" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM66" s="3">
+      <c r="AL66" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM66" s="1">
         <v>1.8</v>
       </c>
       <c r="AN66" s="1">
+        <v>102.2</v>
+      </c>
+      <c r="AO66" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="67" ht="35.6" spans="1:40">
+    <row r="67" ht="35.6" spans="1:41">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D67" s="1">
         <v>1960</v>
@@ -9297,10 +9496,10 @@
         <v>0.7</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N67" s="2">
         <v>15113</v>
@@ -9381,18 +9580,21 @@
         <v>0.1</v>
       </c>
       <c r="AN67" s="1">
+        <v>115.5</v>
+      </c>
+      <c r="AO67" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="68" ht="35.6" spans="1:40">
+    <row r="68" ht="35.6" spans="1:41">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D68" s="1">
         <v>1960</v>
@@ -9420,10 +9622,10 @@
         <v>0.7</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N68" s="2">
         <v>5225</v>
@@ -9504,18 +9706,21 @@
         <v>0.2</v>
       </c>
       <c r="AN68" s="1">
+        <v>112.6</v>
+      </c>
+      <c r="AO68" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="69" ht="35.6" spans="1:40">
+    <row r="69" ht="35.6" spans="1:41">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D69" s="1">
         <v>1960</v>
@@ -9543,10 +9748,10 @@
         <v>0.7</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N69" s="2">
         <v>2179</v>
@@ -9627,18 +9832,21 @@
         <v>0.3</v>
       </c>
       <c r="AN69" s="1">
+        <v>110.4</v>
+      </c>
+      <c r="AO69" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="70" ht="35.6" spans="1:40">
+    <row r="70" ht="35.6" spans="1:41">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D70" s="1">
         <v>1960</v>
@@ -9666,10 +9874,10 @@
         <v>0.7</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N70" s="2">
         <v>956.5</v>
@@ -9750,18 +9958,21 @@
         <v>0.4</v>
       </c>
       <c r="AN70" s="1">
+        <v>108.6</v>
+      </c>
+      <c r="AO70" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="71" ht="35.6" spans="1:40">
+    <row r="71" ht="35.6" spans="1:41">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D71" s="1">
         <v>1960</v>
@@ -9789,10 +10000,10 @@
         <v>0.7</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N71" s="2">
         <v>460.1</v>
@@ -9873,18 +10084,21 @@
         <v>0.4</v>
       </c>
       <c r="AN71" s="1">
+        <v>107.2</v>
+      </c>
+      <c r="AO71" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="72" ht="35.6" spans="1:40">
+    <row r="72" ht="35.6" spans="1:41">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D72" s="1">
         <v>1960</v>
@@ -9912,10 +10126,10 @@
         <v>0.7</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N72" s="2">
         <v>233.1</v>
@@ -9996,18 +10210,21 @@
         <v>0.5</v>
       </c>
       <c r="AN72" s="1">
+        <v>106.2</v>
+      </c>
+      <c r="AO72" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="73" ht="35.6" spans="1:40">
+    <row r="73" ht="35.6" spans="1:41">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D73" s="1">
         <v>1960</v>
@@ -10035,10 +10252,10 @@
         <v>0.7</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N73" s="2">
         <v>109.9</v>
@@ -10119,18 +10336,21 @@
         <v>0.5</v>
       </c>
       <c r="AN73" s="1">
+        <v>105.2</v>
+      </c>
+      <c r="AO73" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="74" ht="35.6" spans="1:40">
+    <row r="74" ht="35.6" spans="1:41">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D74" s="1">
         <v>1960</v>
@@ -10158,10 +10378,10 @@
         <v>0.7</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N74" s="2">
         <v>45.48</v>
@@ -10242,18 +10462,21 @@
         <v>0.5</v>
       </c>
       <c r="AN74" s="1">
+        <v>104.2</v>
+      </c>
+      <c r="AO74" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="75" ht="35.6" spans="1:40">
+    <row r="75" ht="35.6" spans="1:41">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D75" s="1">
         <v>1960</v>
@@ -10281,10 +10504,10 @@
         <v>0.7</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N75" s="2">
         <v>19.83</v>
@@ -10365,18 +10588,21 @@
         <v>0.5</v>
       </c>
       <c r="AN75" s="1">
+        <v>103.6</v>
+      </c>
+      <c r="AO75" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="76" ht="35.6" spans="1:40">
+    <row r="76" ht="35.6" spans="1:41">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D76" s="1">
         <v>1960</v>
@@ -10404,10 +10630,10 @@
         <v>0.7</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N76" s="2">
         <v>9.136</v>
@@ -10488,18 +10714,21 @@
         <v>0.5</v>
       </c>
       <c r="AN76" s="1">
+        <v>103.1</v>
+      </c>
+      <c r="AO76" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="77" ht="35.6" spans="1:40">
+    <row r="77" ht="35.6" spans="1:41">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D77" s="1">
         <v>1960</v>
@@ -10527,10 +10756,10 @@
         <v>0.7</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N77" s="2">
         <v>3.734</v>
@@ -10611,18 +10840,21 @@
         <v>0.5</v>
       </c>
       <c r="AN77" s="1">
+        <v>102.8</v>
+      </c>
+      <c r="AO77" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="78" ht="35.6" spans="1:40">
+    <row r="78" ht="35.6" spans="1:41">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D78" s="1">
         <v>1960</v>
@@ -10650,10 +10882,10 @@
         <v>0.7</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N78" s="2">
         <v>1.23</v>
@@ -10734,18 +10966,21 @@
         <v>0.4</v>
       </c>
       <c r="AN78" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="AO78" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="79" ht="35.6" spans="1:40">
+    <row r="79" ht="35.6" spans="1:41">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D79" s="1">
         <v>1960</v>
@@ -10773,10 +11008,10 @@
         <v>0.7</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N79" s="2">
         <v>0.3532</v>
@@ -10857,18 +11092,21 @@
         <v>0.3</v>
       </c>
       <c r="AN79" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO79" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="80" ht="35.6" spans="1:40">
+    <row r="80" ht="35.6" spans="1:41">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D80" s="1">
         <v>1960</v>
@@ -10896,10 +11134,10 @@
         <v>0.7</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N80" s="2">
         <v>0.1083</v>
@@ -10980,18 +11218,21 @@
         <v>0.2</v>
       </c>
       <c r="AN80" s="1">
+        <v>102.2</v>
+      </c>
+      <c r="AO80" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="81" ht="35.6" spans="1:40">
+    <row r="81" ht="35.6" spans="1:41">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D81" s="1">
         <v>1960</v>
@@ -11019,10 +11260,10 @@
         <v>0.7</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N81" s="2">
         <v>0.0291</v>
@@ -11103,18 +11344,21 @@
         <v>0</v>
       </c>
       <c r="AN81" s="1">
+        <v>102.2</v>
+      </c>
+      <c r="AO81" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="82" ht="35.6" spans="1:40">
+    <row r="82" ht="35.6" spans="1:41">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D82" s="1">
         <v>1960</v>
@@ -11142,10 +11386,10 @@
         <v>0.7</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N82" s="2">
         <v>0.007082</v>
@@ -11226,18 +11470,21 @@
         <v>0.2</v>
       </c>
       <c r="AN82" s="1">
+        <v>102.1</v>
+      </c>
+      <c r="AO82" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="83" ht="35.6" spans="1:40">
+    <row r="83" ht="35.6" spans="1:41">
       <c r="A83" s="1">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D83" s="1">
         <v>1960</v>
@@ -11265,102 +11512,105 @@
         <v>0.7</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N83" s="2">
         <v>0.0003741</v>
       </c>
-      <c r="O83" s="3">
+      <c r="O83" s="1">
         <v>4.3e-5</v>
       </c>
-      <c r="P83" s="3">
+      <c r="P83" s="1">
         <v>9.9</v>
       </c>
-      <c r="Q83" s="3">
+      <c r="Q83" s="1">
         <v>8.2</v>
       </c>
-      <c r="R83" s="3">
+      <c r="R83" s="1">
         <v>13.1</v>
       </c>
-      <c r="S83" s="3">
+      <c r="S83" s="1">
         <v>11.7</v>
       </c>
-      <c r="T83" s="3">
-        <v>0</v>
-      </c>
-      <c r="U83" s="3">
+      <c r="T83" s="1">
+        <v>0</v>
+      </c>
+      <c r="U83" s="1">
         <v>9.5</v>
       </c>
-      <c r="V83" s="3">
+      <c r="V83" s="1">
         <v>6.5</v>
       </c>
-      <c r="W83" s="3">
+      <c r="W83" s="1">
         <v>8.3</v>
       </c>
-      <c r="X83" s="3">
+      <c r="X83" s="1">
         <v>6</v>
       </c>
-      <c r="Y83" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z83" s="3">
+      <c r="Y83" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="1">
         <v>6.7</v>
       </c>
-      <c r="AA83" s="3">
+      <c r="AA83" s="1">
         <v>9.6</v>
       </c>
-      <c r="AB83" s="3">
+      <c r="AB83" s="1">
         <v>3.9</v>
       </c>
-      <c r="AC83" s="3">
+      <c r="AC83" s="1">
         <v>3.3</v>
       </c>
-      <c r="AD83" s="3">
+      <c r="AD83" s="1">
         <v>6.4</v>
       </c>
-      <c r="AE83" s="3">
+      <c r="AE83" s="1">
         <v>7.5</v>
       </c>
-      <c r="AF83" s="3">
+      <c r="AF83" s="1">
         <v>2.5</v>
       </c>
-      <c r="AG83" s="3">
+      <c r="AG83" s="1">
         <v>2.3</v>
       </c>
-      <c r="AH83" s="3">
+      <c r="AH83" s="1">
         <v>1.4</v>
       </c>
-      <c r="AI83" s="3">
+      <c r="AI83" s="1">
         <v>5.6</v>
       </c>
-      <c r="AJ83" s="3">
+      <c r="AJ83" s="1">
         <v>0.6</v>
       </c>
-      <c r="AK83" s="3">
+      <c r="AK83" s="1">
         <v>1.3</v>
       </c>
-      <c r="AL83" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM83" s="3">
+      <c r="AL83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM83" s="1">
         <v>0.8</v>
       </c>
       <c r="AN83" s="1">
+        <v>102.1</v>
+      </c>
+      <c r="AO83" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="84" ht="35.6" spans="1:40">
+    <row r="84" ht="35.6" spans="1:41">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D84" s="1">
         <v>1960</v>
@@ -11388,10 +11638,10 @@
         <v>0.7</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N84" s="2">
         <v>11591</v>
@@ -11472,18 +11722,21 @@
         <v>0.1</v>
       </c>
       <c r="AN84" s="1">
+        <v>116.9</v>
+      </c>
+      <c r="AO84" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="85" ht="35.6" spans="1:40">
+    <row r="85" ht="35.6" spans="1:41">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D85" s="1">
         <v>1960</v>
@@ -11511,10 +11764,10 @@
         <v>0.7</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N85" s="2">
         <v>4020</v>
@@ -11595,18 +11848,21 @@
         <v>0.2</v>
       </c>
       <c r="AN85" s="1">
+        <v>113.1</v>
+      </c>
+      <c r="AO85" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="86" ht="35.6" spans="1:40">
+    <row r="86" ht="35.6" spans="1:41">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D86" s="1">
         <v>1960</v>
@@ -11634,10 +11890,10 @@
         <v>0.7</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N86" s="2">
         <v>1555</v>
@@ -11718,18 +11974,21 @@
         <v>0.3</v>
       </c>
       <c r="AN86" s="1">
+        <v>110.2</v>
+      </c>
+      <c r="AO86" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="87" ht="35.6" spans="1:40">
+    <row r="87" ht="35.6" spans="1:41">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D87" s="1">
         <v>1960</v>
@@ -11757,10 +12016,10 @@
         <v>0.7</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N87" s="2">
         <v>664.2</v>
@@ -11841,18 +12100,21 @@
         <v>0.4</v>
       </c>
       <c r="AN87" s="1">
+        <v>108.1</v>
+      </c>
+      <c r="AO87" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="88" ht="35.6" spans="1:40">
+    <row r="88" ht="35.6" spans="1:41">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D88" s="1">
         <v>1960</v>
@@ -11880,10 +12142,10 @@
         <v>0.7</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N88" s="2">
         <v>293.3</v>
@@ -11964,18 +12226,21 @@
         <v>0.5</v>
       </c>
       <c r="AN88" s="1">
+        <v>106.6</v>
+      </c>
+      <c r="AO88" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="89" ht="35.6" spans="1:40">
+    <row r="89" ht="35.6" spans="1:41">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D89" s="1">
         <v>1960</v>
@@ -12003,10 +12268,10 @@
         <v>0.7</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N89" s="2">
         <v>135</v>
@@ -12087,18 +12352,21 @@
         <v>0.5</v>
       </c>
       <c r="AN89" s="1">
+        <v>105.4</v>
+      </c>
+      <c r="AO89" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="90" ht="35.6" spans="1:40">
+    <row r="90" ht="35.6" spans="1:41">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D90" s="1">
         <v>1960</v>
@@ -12126,10 +12394,10 @@
         <v>0.7</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N90" s="2">
         <v>56.4</v>
@@ -12210,18 +12478,21 @@
         <v>0.6</v>
       </c>
       <c r="AN90" s="1">
+        <v>104.4</v>
+      </c>
+      <c r="AO90" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="91" ht="35.6" spans="1:40">
+    <row r="91" ht="35.6" spans="1:41">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D91" s="1">
         <v>1960</v>
@@ -12249,10 +12520,10 @@
         <v>0.7</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N91" s="2">
         <v>20.13</v>
@@ -12333,18 +12604,21 @@
         <v>0.6</v>
       </c>
       <c r="AN91" s="1">
+        <v>103.5</v>
+      </c>
+      <c r="AO91" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="92" ht="35.6" spans="1:40">
+    <row r="92" ht="35.6" spans="1:41">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D92" s="1">
         <v>1960</v>
@@ -12372,10 +12646,10 @@
         <v>0.7</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N92" s="2">
         <v>6.279</v>
@@ -12456,18 +12730,21 @@
         <v>0.6</v>
       </c>
       <c r="AN92" s="1">
+        <v>102.9</v>
+      </c>
+      <c r="AO92" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="93" ht="35.6" spans="1:40">
+    <row r="93" ht="35.6" spans="1:41">
       <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D93" s="1">
         <v>1960</v>
@@ -12495,10 +12772,10 @@
         <v>0.7</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N93" s="2">
         <v>1.91</v>
@@ -12579,18 +12856,21 @@
         <v>0.6</v>
       </c>
       <c r="AN93" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="AO93" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="94" ht="35.6" spans="1:40">
+    <row r="94" ht="35.6" spans="1:41">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D94" s="1">
         <v>1960</v>
@@ -12618,10 +12898,10 @@
         <v>0.7</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N94" s="2">
         <v>0.6805</v>
@@ -12702,18 +12982,21 @@
         <v>0.6</v>
       </c>
       <c r="AN94" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO94" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="95" ht="35.6" spans="1:40">
+    <row r="95" ht="35.6" spans="1:41">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D95" s="1">
         <v>1960</v>
@@ -12741,10 +13024,10 @@
         <v>0.7</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N95" s="2">
         <v>0.2176</v>
@@ -12825,18 +13108,21 @@
         <v>0.6</v>
       </c>
       <c r="AN95" s="1">
+        <v>102.1</v>
+      </c>
+      <c r="AO95" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="96" ht="35.6" spans="1:40">
+    <row r="96" ht="35.6" spans="1:41">
       <c r="A96" s="1">
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D96" s="1">
         <v>1960</v>
@@ -12864,10 +13150,10 @@
         <v>0.7</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N96" s="2">
         <v>0.04463</v>
@@ -12948,18 +13234,21 @@
         <v>0.5</v>
       </c>
       <c r="AN96" s="1">
+        <v>102</v>
+      </c>
+      <c r="AO96" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="97" ht="35.6" spans="1:40">
+    <row r="97" ht="35.6" spans="1:41">
       <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D97" s="1">
         <v>1960</v>
@@ -12987,10 +13276,10 @@
         <v>0.7</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N97" s="2">
         <v>0.006544</v>
@@ -13071,18 +13360,21 @@
         <v>0.3</v>
       </c>
       <c r="AN97" s="1">
+        <v>102</v>
+      </c>
+      <c r="AO97" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="98" ht="35.6" spans="1:40">
+    <row r="98" ht="35.6" spans="1:41">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D98" s="1">
         <v>1960</v>
@@ -13110,102 +13402,105 @@
         <v>0.7</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N98" s="2">
         <v>0.0003747</v>
       </c>
-      <c r="O98" s="3">
+      <c r="O98" s="1">
         <v>6.15e-5</v>
       </c>
-      <c r="P98" s="3">
+      <c r="P98" s="1">
         <v>12.9</v>
       </c>
-      <c r="Q98" s="3">
+      <c r="Q98" s="1">
         <v>10.7</v>
       </c>
-      <c r="R98" s="3">
+      <c r="R98" s="1">
         <v>17.5</v>
       </c>
-      <c r="S98" s="3">
+      <c r="S98" s="1">
         <v>17</v>
       </c>
-      <c r="T98" s="3">
-        <v>0</v>
-      </c>
-      <c r="U98" s="3">
+      <c r="T98" s="1">
+        <v>0</v>
+      </c>
+      <c r="U98" s="1">
         <v>12.7</v>
       </c>
-      <c r="V98" s="3">
+      <c r="V98" s="1">
         <v>6.5</v>
       </c>
-      <c r="W98" s="3">
-        <v>0</v>
-      </c>
-      <c r="X98" s="3">
+      <c r="W98" s="1">
+        <v>0</v>
+      </c>
+      <c r="X98" s="1">
         <v>8.9</v>
       </c>
-      <c r="Y98" s="3">
+      <c r="Y98" s="1">
         <v>11</v>
       </c>
-      <c r="Z98" s="3">
+      <c r="Z98" s="1">
         <v>12</v>
       </c>
-      <c r="AA98" s="3">
+      <c r="AA98" s="1">
         <v>21.8</v>
       </c>
-      <c r="AB98" s="3">
+      <c r="AB98" s="1">
         <v>0.2</v>
       </c>
-      <c r="AC98" s="3">
+      <c r="AC98" s="1">
         <v>6.1</v>
       </c>
-      <c r="AD98" s="3">
+      <c r="AD98" s="1">
         <v>5.3</v>
       </c>
-      <c r="AE98" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF98" s="3">
+      <c r="AE98" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF98" s="1">
         <v>0.1</v>
       </c>
-      <c r="AG98" s="3">
+      <c r="AG98" s="1">
         <v>4.2</v>
       </c>
-      <c r="AH98" s="3">
+      <c r="AH98" s="1">
         <v>3.9</v>
       </c>
-      <c r="AI98" s="3">
+      <c r="AI98" s="1">
         <v>0.9</v>
       </c>
-      <c r="AJ98" s="3">
+      <c r="AJ98" s="1">
         <v>1</v>
       </c>
-      <c r="AK98" s="3">
+      <c r="AK98" s="1">
         <v>1.5</v>
       </c>
-      <c r="AL98" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM98" s="3">
+      <c r="AL98" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM98" s="1">
         <v>0.1</v>
       </c>
       <c r="AN98" s="1">
+        <v>101.9</v>
+      </c>
+      <c r="AO98" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="99" ht="35.6" spans="1:40">
+    <row r="99" ht="35.6" spans="1:41">
       <c r="A99" s="1">
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D99" s="1">
         <v>1960</v>
@@ -13233,10 +13528,10 @@
         <v>0.7</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N99" s="2">
         <v>7154</v>
@@ -13317,18 +13612,21 @@
         <v>0.1</v>
       </c>
       <c r="AN99" s="1">
+        <v>116.2</v>
+      </c>
+      <c r="AO99" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="100" ht="35.6" spans="1:40">
+    <row r="100" ht="35.6" spans="1:41">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D100" s="1">
         <v>1960</v>
@@ -13356,10 +13654,10 @@
         <v>0.7</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N100" s="2">
         <v>2263</v>
@@ -13440,18 +13738,21 @@
         <v>0.3</v>
       </c>
       <c r="AN100" s="1">
+        <v>111.6</v>
+      </c>
+      <c r="AO100" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="101" ht="35.6" spans="1:40">
+    <row r="101" ht="35.6" spans="1:41">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D101" s="1">
         <v>1960</v>
@@ -13479,10 +13780,10 @@
         <v>0.7</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N101" s="2">
         <v>734.7</v>
@@ -13563,18 +13864,21 @@
         <v>0.4</v>
       </c>
       <c r="AN101" s="1">
+        <v>108.5</v>
+      </c>
+      <c r="AO101" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="102" ht="35.6" spans="1:40">
+    <row r="102" ht="35.6" spans="1:41">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D102" s="1">
         <v>1960</v>
@@ -13602,10 +13906,10 @@
         <v>0.7</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N102" s="2">
         <v>268.5</v>
@@ -13686,18 +13990,21 @@
         <v>0.5</v>
       </c>
       <c r="AN102" s="1">
+        <v>106.4</v>
+      </c>
+      <c r="AO102" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="103" ht="35.6" spans="1:40">
+    <row r="103" ht="35.6" spans="1:41">
       <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D103" s="1">
         <v>1960</v>
@@ -13725,10 +14032,10 @@
         <v>0.7</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N103" s="2">
         <v>98.47</v>
@@ -13809,18 +14116,21 @@
         <v>0.6</v>
       </c>
       <c r="AN103" s="1">
+        <v>104.9</v>
+      </c>
+      <c r="AO103" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="104" ht="35.6" spans="1:40">
+    <row r="104" ht="35.6" spans="1:41">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D104" s="1">
         <v>1960</v>
@@ -13848,10 +14158,10 @@
         <v>0.7</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N104" s="2">
         <v>38.31</v>
@@ -13932,18 +14242,21 @@
         <v>0.7</v>
       </c>
       <c r="AN104" s="1">
+        <v>103.9</v>
+      </c>
+      <c r="AO104" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="105" ht="35.6" spans="1:40">
+    <row r="105" ht="35.6" spans="1:41">
       <c r="A105" s="1">
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D105" s="1">
         <v>1960</v>
@@ -13971,10 +14284,10 @@
         <v>0.7</v>
       </c>
       <c r="L105" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N105" s="2">
         <v>14.53</v>
@@ -14055,18 +14368,21 @@
         <v>0.7</v>
       </c>
       <c r="AN105" s="1">
+        <v>103.2</v>
+      </c>
+      <c r="AO105" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="106" ht="35.6" spans="1:40">
+    <row r="106" ht="35.6" spans="1:41">
       <c r="A106" s="1">
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D106" s="1">
         <v>1960</v>
@@ -14094,10 +14410,10 @@
         <v>0.7</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N106" s="2">
         <v>5.643</v>
@@ -14178,18 +14494,21 @@
         <v>0.8</v>
       </c>
       <c r="AN106" s="1">
+        <v>102.7</v>
+      </c>
+      <c r="AO106" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="107" ht="35.6" spans="1:40">
+    <row r="107" ht="35.6" spans="1:41">
       <c r="A107" s="1">
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D107" s="1">
         <v>1960</v>
@@ -14217,10 +14536,10 @@
         <v>0.7</v>
       </c>
       <c r="L107" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N107" s="2">
         <v>1.787</v>
@@ -14301,18 +14620,21 @@
         <v>0.9</v>
       </c>
       <c r="AN107" s="1">
+        <v>102.3</v>
+      </c>
+      <c r="AO107" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="108" ht="35.6" spans="1:40">
+    <row r="108" ht="35.6" spans="1:41">
       <c r="A108" s="1">
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D108" s="1">
         <v>1960</v>
@@ -14340,10 +14662,10 @@
         <v>0.7</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N108" s="2">
         <v>0.3752</v>
@@ -14424,18 +14746,21 @@
         <v>0.9</v>
       </c>
       <c r="AN108" s="1">
+        <v>102</v>
+      </c>
+      <c r="AO108" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="109" ht="35.6" spans="1:40">
+    <row r="109" ht="35.6" spans="1:41">
       <c r="A109" s="1">
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D109" s="1">
         <v>1960</v>
@@ -14463,10 +14788,10 @@
         <v>0.7</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N109" s="2">
         <v>0.07923</v>
@@ -14547,18 +14872,21 @@
         <v>1</v>
       </c>
       <c r="AN109" s="1">
+        <v>101.8</v>
+      </c>
+      <c r="AO109" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="110" ht="35.6" spans="1:40">
+    <row r="110" ht="35.6" spans="1:41">
       <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D110" s="1">
         <v>1960</v>
@@ -14586,10 +14914,10 @@
         <v>0.7</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N110" s="2">
         <v>0.01048</v>
@@ -14670,18 +14998,21 @@
         <v>1</v>
       </c>
       <c r="AN110" s="1">
+        <v>101.7</v>
+      </c>
+      <c r="AO110" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="111" ht="35.6" spans="1:40">
+    <row r="111" ht="35.6" spans="1:41">
       <c r="A111" s="1">
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D111" s="1">
         <v>1960</v>
@@ -14709,90 +15040,93 @@
         <v>0.7</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N111" s="2">
         <v>0.0003314</v>
       </c>
-      <c r="O111" s="3">
+      <c r="O111" s="1">
         <v>6.26e-5</v>
       </c>
-      <c r="P111" s="3">
+      <c r="P111" s="1">
         <v>16.7</v>
       </c>
-      <c r="Q111" s="3">
+      <c r="Q111" s="1">
         <v>12.4</v>
       </c>
-      <c r="R111" s="3">
+      <c r="R111" s="1">
         <v>20.6</v>
       </c>
-      <c r="S111" s="3">
+      <c r="S111" s="1">
         <v>21.4</v>
       </c>
-      <c r="T111" s="3">
+      <c r="T111" s="1">
         <v>15.1</v>
       </c>
-      <c r="U111" s="3">
+      <c r="U111" s="1">
         <v>15</v>
       </c>
-      <c r="V111" s="3">
+      <c r="V111" s="1">
         <v>6.5</v>
       </c>
-      <c r="W111" s="3">
-        <v>0</v>
-      </c>
-      <c r="X111" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y111" s="3">
+      <c r="W111" s="1">
+        <v>0</v>
+      </c>
+      <c r="X111" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y111" s="1">
         <v>14.9</v>
       </c>
-      <c r="Z111" s="3">
+      <c r="Z111" s="1">
         <v>17.8</v>
       </c>
-      <c r="AA111" s="3">
+      <c r="AA111" s="1">
         <v>9.2</v>
       </c>
-      <c r="AB111" s="3">
+      <c r="AB111" s="1">
         <v>0.2</v>
       </c>
-      <c r="AC111" s="3">
+      <c r="AC111" s="1">
         <v>10.3</v>
       </c>
-      <c r="AD111" s="3">
+      <c r="AD111" s="1">
         <v>8.2</v>
       </c>
-      <c r="AE111" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF111" s="3">
+      <c r="AE111" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF111" s="1">
         <v>3.4</v>
       </c>
-      <c r="AG111" s="3">
+      <c r="AG111" s="1">
         <v>4.9</v>
       </c>
-      <c r="AH111" s="3">
+      <c r="AH111" s="1">
         <v>10.2</v>
       </c>
-      <c r="AI111" s="3">
+      <c r="AI111" s="1">
         <v>0.9</v>
       </c>
-      <c r="AJ111" s="3">
+      <c r="AJ111" s="1">
         <v>4.2</v>
       </c>
-      <c r="AK111" s="3">
+      <c r="AK111" s="1">
         <v>1.6</v>
       </c>
-      <c r="AL111" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM111" s="3">
+      <c r="AL111" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM111" s="1">
         <v>0.9</v>
       </c>
       <c r="AN111" s="1">
+        <v>101.6</v>
+      </c>
+      <c r="AO111" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update in unpolarized jets
add normalization uncertainty for D0 data
better format CDF data table
</commit_message>
<xml_diff>
--- a/jets/expdata/10001.xlsx
+++ b/jets/expdata/10001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17020" tabRatio="500"/>
+    <workbookView windowHeight="17880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <t>%-sys05_c</t>
   </si>
   <si>
-    <t>%-sys06_c</t>
+    <t>%-norm_c</t>
   </si>
   <si>
     <t>%-sys07_c</t>
@@ -156,11 +156,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -176,11 +176,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,10 +190,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -205,9 +212,100 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,106 +320,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,7 +336,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,79 +474,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,55 +492,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,25 +510,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,20 +545,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -578,27 +575,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -627,151 +607,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -780,7 +780,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1104,10 +1104,10 @@
   <sheetPr/>
   <dimension ref="A1:AO123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" topLeftCell="AH1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AN1" sqref="AN$1:AN$1048576"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71120689655172" defaultRowHeight="24.4"/>
@@ -15299,7 +15299,7 @@
       <c r="P123" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>

</xml_diff>